<commit_message>
Test Cases for Doctor Registration and Login
</commit_message>
<xml_diff>
--- a/Health-care System Test Cases Writing/Login.xlsx
+++ b/Health-care System Test Cases Writing/Login.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\SQA Resources\Test Cases\Health-care System\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SQA and Cyber Security Course\TestCase Github\Test-Cases\Health-care System Test Cases Writing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC9F8D52-A635-4C47-A30A-DC858F2F2B23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43C5E23-1257-4B69-B92A-D102A192383C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="64">
   <si>
     <t>PASS</t>
   </si>
@@ -209,6 +209,9 @@
   </si>
   <si>
     <t>InvalidUserNameAndValidPassword</t>
+  </si>
+  <si>
+    <t>http://localhost/Health-care-system/pindex.php</t>
   </si>
 </sst>
 </file>
@@ -548,6 +551,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -564,12 +573,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1271,7 +1274,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1290,10 +1293,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="37"/>
+      <c r="B1" s="39"/>
       <c r="C1" s="1" t="s">
         <v>34</v>
       </c>
@@ -1309,16 +1312,16 @@
       <c r="G1" s="5">
         <v>44446</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="37"/>
+      <c r="I1" s="39"/>
     </row>
     <row r="2" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="37"/>
+      <c r="B2" s="39"/>
       <c r="C2" s="2" t="s">
         <v>36</v>
       </c>
@@ -1343,8 +1346,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="39"/>
-      <c r="B3" s="37"/>
+      <c r="A3" s="41"/>
+      <c r="B3" s="39"/>
       <c r="C3" s="2"/>
       <c r="D3" s="9" t="s">
         <v>12</v>
@@ -1367,10 +1370,10 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="39" t="s">
+      <c r="A4" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="37"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="2"/>
       <c r="D4" s="9" t="s">
         <v>15</v>
@@ -1391,15 +1394,15 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="37"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="39"/>
       <c r="H5" s="12" t="s">
         <v>19</v>
       </c>
@@ -1460,7 +1463,7 @@
       <c r="H7" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="I7" s="42" t="s">
+      <c r="I7" s="36" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1470,7 +1473,9 @@
       <c r="C8" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="28"/>
+      <c r="D8" s="36" t="s">
+        <v>63</v>
+      </c>
       <c r="E8" s="16" t="s">
         <v>42</v>
       </c>
@@ -1553,7 +1558,7 @@
       <c r="H12" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="I12" s="42" t="s">
+      <c r="I12" s="36" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1614,7 +1619,7 @@
       <c r="H15" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="I15" s="42" t="s">
+      <c r="I15" s="36" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1675,7 +1680,7 @@
       <c r="H18" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="I18" s="43" t="s">
+      <c r="I18" s="37" t="s">
         <v>62</v>
       </c>
     </row>
@@ -3003,8 +3008,9 @@
     <hyperlink ref="I15" r:id="rId2" xr:uid="{1C25A5EB-8960-44C3-85E0-FFBEEA3918F1}"/>
     <hyperlink ref="I12" r:id="rId3" xr:uid="{A92349BB-70EE-43E8-8261-38211EFCE652}"/>
     <hyperlink ref="I18" r:id="rId4" xr:uid="{E6376FE9-A1F2-4465-8609-0EC7CAE0A8C5}"/>
+    <hyperlink ref="D8" r:id="rId5" xr:uid="{62363B88-6D3C-4249-A1B9-8131D04AC3B6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId5"/>
+  <pageSetup orientation="landscape" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>